<commit_message>
hibernate INFO issue resolved
</commit_message>
<xml_diff>
--- a/Payments-template-example.xlsx
+++ b/Payments-template-example.xlsx
@@ -223,10 +223,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.34"/>

</xml_diff>